<commit_message>
Fixed an issue with digit_count
</commit_message>
<xml_diff>
--- a/file.xlsx
+++ b/file.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissabenefer/PycharmProjects/Bens/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissabenefer/PycharmProjects/BenfordsLaw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2468AFC2-6113-7241-841B-7BFF2C6A488C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7304D66-A5A7-8142-8190-6A66E87832D3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="460" yWindow="5700" windowWidth="28040" windowHeight="16340" xr2:uid="{97B0E444-2F5F-A845-A70D-29E150DA2C2C}"/>
+    <workbookView xWindow="460" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{97B0E444-2F5F-A845-A70D-29E150DA2C2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +60,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -68,12 +68,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19807CE6-5D03-9347-82F5-F38D98DE131C}">
-  <dimension ref="A1:A41"/>
+  <dimension ref="A1:A59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:A41"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -402,203 +434,293 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>100</v>
+      <c r="A2" s="1">
+        <v>1680380</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>200</v>
+      <c r="A3" s="1">
+        <v>1204</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>300</v>
+      <c r="A4" s="1">
+        <v>40532</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>400</v>
+      <c r="A5" s="1">
+        <v>210135</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>500</v>
+      <c r="A6" s="1">
+        <v>45346</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>600</v>
+      <c r="A7" s="1">
+        <v>21858</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>700</v>
+      <c r="A8" s="1">
+        <v>1165986</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>800</v>
+      <c r="A9" s="1">
+        <v>27601</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>900</v>
+      <c r="A10" s="1">
+        <v>191220</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>900</v>
+      <c r="A11" s="1">
+        <v>1009503</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>900</v>
+      <c r="A12" s="1">
+        <v>28896</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>900</v>
+      <c r="A13" s="1">
+        <v>136261</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>900</v>
+      <c r="A14" s="1">
+        <v>179595</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>900</v>
+      <c r="A15" s="1">
+        <v>19001</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>900</v>
+      <c r="A16" s="1">
+        <v>905828</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>900</v>
+      <c r="A17" s="1">
+        <v>152790</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>900</v>
+      <c r="A18" s="1">
+        <v>68195</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>900</v>
+      <c r="A19" s="1">
+        <v>32317</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>900</v>
+      <c r="A20" s="1">
+        <v>9992236</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>900</v>
+      <c r="A21" s="1">
+        <v>156343</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>900</v>
+      <c r="A22" s="1">
+        <v>261282</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>900</v>
+      <c r="A23" s="1">
+        <v>17118</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>900</v>
+      <c r="A24" s="1">
+        <v>91361</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>900</v>
+      <c r="A25" s="1">
+        <v>281814</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>900</v>
+      <c r="A26" s="1">
+        <v>8663</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>900</v>
+      <c r="A27" s="1">
+        <v>13226</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>900</v>
+      <c r="A28" s="1">
+        <v>438390</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>900</v>
+      <c r="A29" s="1">
+        <v>137485</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>900</v>
+      <c r="A30" s="1">
+        <v>102249</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>900</v>
+      <c r="A31" s="1">
+        <v>3185516</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>900</v>
+      <c r="A32" s="1">
+        <v>405889</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>900</v>
+      <c r="A33" s="1">
+        <v>19749</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>900</v>
+      <c r="A34" s="1">
+        <v>2422847</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>900</v>
+      <c r="A35" s="1">
+        <v>1586465</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>900</v>
+      <c r="A36" s="1">
+        <v>64521</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>900</v>
+      <c r="A37" s="1">
+        <v>2183239</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>900</v>
+      <c r="A38" s="1">
+        <v>3296045</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>900</v>
+      <c r="A39" s="1">
+        <v>870393</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>900</v>
+      <c r="A40" s="1">
+        <v>780558</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>900</v>
+      <c r="A41" s="1">
+        <v>281879</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>762511</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>448244</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>1931026</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>270462</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>181984</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>3228</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>43991</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>452698</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>488281</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>553217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>99464</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>65682</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>16089</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>473891</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>55374</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>843310</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>216291</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" s="2">
+        <v>81994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>